<commit_message>
included M1 Pro and M1 Max
</commit_message>
<xml_diff>
--- a/gpu/gpu_comparison.xlsx
+++ b/gpu/gpu_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library\Github\benchmark\gpu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DA0B8D-E58A-4D0E-B6CD-1AA8D7463BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F171782-B430-4E48-BEFC-57462FCAEE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19935" yWindow="5235" windowWidth="14565" windowHeight="13635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="3270" windowWidth="17760" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
   <si>
     <t>model</t>
   </si>
@@ -120,12 +120,6 @@
     <t>512 MB</t>
   </si>
   <si>
-    <t>22.40 GB/s</t>
-  </si>
-  <si>
-    <t>217.6 GB/s</t>
-  </si>
-  <si>
     <t>Xbox One S</t>
   </si>
   <si>
@@ -138,18 +132,6 @@
     <t>DDR3</t>
   </si>
   <si>
-    <t>68.22 GB/s</t>
-  </si>
-  <si>
-    <t>20.80 GB/s</t>
-  </si>
-  <si>
-    <t>211.2 GB/s</t>
-  </si>
-  <si>
-    <t>176.0 GB/s</t>
-  </si>
-  <si>
     <t>GFLOPS FP32</t>
   </si>
   <si>
@@ -159,9 +141,6 @@
     <t>Lockhard</t>
   </si>
   <si>
-    <t>224.0 GB/s</t>
-  </si>
-  <si>
     <t>CU</t>
   </si>
   <si>
@@ -174,9 +153,6 @@
     <t>10000 MB</t>
   </si>
   <si>
-    <t>560.0 GB/s</t>
-  </si>
-  <si>
     <t>GeForce GTX 960</t>
   </si>
   <si>
@@ -186,10 +162,31 @@
     <t>2048 MB</t>
   </si>
   <si>
-    <t>112.2 GB/s</t>
-  </si>
-  <si>
-    <t>448.0 GB/s</t>
+    <t>Apple M1</t>
+  </si>
+  <si>
+    <t>Apple M1 Pro</t>
+  </si>
+  <si>
+    <t>Apple M1 Max</t>
+  </si>
+  <si>
+    <t>GB/s</t>
+  </si>
+  <si>
+    <t>32000 MB</t>
+  </si>
+  <si>
+    <t>64000 MB</t>
+  </si>
+  <si>
+    <t>LPDDR5</t>
+  </si>
+  <si>
+    <t>164 GT/s</t>
+  </si>
+  <si>
+    <t>82 Gpixel/s</t>
   </si>
 </sst>
 </file>
@@ -205,12 +202,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -225,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -234,6 +243,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -516,22 +539,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:M13"/>
+  <dimension ref="A2:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" customWidth="1"/>
-    <col min="4" max="9" width="8.85546875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="7" style="2" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -560,13 +589,16 @@
         <v>9</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -591,46 +623,48 @@
       <c r="I3" s="2">
         <v>2560</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="3">
         <v>6.2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2">
+      <c r="C4" s="4"/>
+      <c r="D4" s="5">
         <v>24</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="5">
         <v>8</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="5">
         <v>24</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="5">
         <v>8</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="5">
         <v>128</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="2">
-        <v>230.4</v>
-      </c>
-      <c r="L4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K4" s="6">
+        <v>230</v>
+      </c>
+      <c r="L4" s="4">
+        <v>21</v>
+      </c>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -647,7 +681,7 @@
         <v>32</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I5" s="2">
         <v>256</v>
@@ -655,46 +689,49 @@
       <c r="J5" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="3">
         <v>1834</v>
       </c>
-      <c r="L5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="L5">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>2304</v>
       </c>
-      <c r="F6" s="2">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5">
         <v>144</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="5">
         <v>32</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="2">
+      <c r="H6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="5">
         <v>256</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="6">
         <v>4200</v>
       </c>
-      <c r="L6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L6" s="4">
+        <v>218</v>
+      </c>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -719,86 +756,92 @@
       <c r="J7" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="3">
         <v>10290</v>
       </c>
-      <c r="L7" t="s">
-        <v>54</v>
+      <c r="L7">
+        <v>448</v>
       </c>
       <c r="M7">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <v>2048</v>
       </c>
-      <c r="F8" s="2">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5">
         <v>128</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="5">
         <v>32</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="5">
         <v>256</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="6">
         <v>4940</v>
       </c>
-      <c r="L8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="L8" s="4">
+        <v>211</v>
+      </c>
+      <c r="M8" s="4"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="7">
         <v>240</v>
       </c>
-      <c r="F9" s="2">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8">
         <v>16</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="8">
         <v>8</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="8">
         <v>128</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="9">
         <v>240</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="7">
+        <v>23</v>
+      </c>
+      <c r="M9" s="7"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10">
         <v>768</v>
@@ -810,27 +853,27 @@
         <v>16</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I10" s="2">
         <v>256</v>
       </c>
       <c r="J10" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1400</v>
+      </c>
+      <c r="L10">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>36</v>
       </c>
-      <c r="K10" s="2">
-        <v>1400</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="B11" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" t="s">
-        <v>43</v>
       </c>
       <c r="C11">
         <v>1280</v>
@@ -842,7 +885,7 @@
         <v>32</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I11" s="2">
         <v>128</v>
@@ -850,22 +893,22 @@
       <c r="J11" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="3">
         <v>4006</v>
       </c>
-      <c r="L11" t="s">
-        <v>44</v>
+      <c r="L11">
+        <v>224</v>
       </c>
       <c r="M11">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C12">
         <v>3328</v>
@@ -876,8 +919,8 @@
       <c r="G12" s="2">
         <v>64</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>48</v>
+      <c r="H12" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="I12" s="2">
         <v>320</v>
@@ -885,22 +928,22 @@
       <c r="J12" t="s">
         <v>24</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="3">
         <v>12150</v>
       </c>
-      <c r="L12" t="s">
-        <v>49</v>
+      <c r="L12">
+        <v>560</v>
       </c>
       <c r="M12">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C13">
         <v>1024</v>
@@ -911,8 +954,8 @@
       <c r="G13" s="2">
         <v>32</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>52</v>
+      <c r="H13" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="I13" s="2">
         <v>128</v>
@@ -920,11 +963,103 @@
       <c r="J13" t="s">
         <v>14</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="3">
         <v>2413</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4">
+        <v>1024</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5">
+        <v>8</v>
+      </c>
+      <c r="F14" s="5">
+        <v>128</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" s="5"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="6">
+        <v>2600</v>
+      </c>
+      <c r="L14" s="4">
+        <v>70</v>
+      </c>
+      <c r="M14" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15">
+        <v>2048</v>
+      </c>
+      <c r="E15" s="2">
+        <v>16</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" s="2">
+        <v>256</v>
+      </c>
+      <c r="J15" t="s">
+        <v>51</v>
+      </c>
+      <c r="K15" s="3">
+        <v>5200</v>
+      </c>
+      <c r="L15">
+        <v>200</v>
+      </c>
+      <c r="N15" t="s">
+        <v>52</v>
+      </c>
+      <c r="O15" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16">
+        <v>4096</v>
+      </c>
+      <c r="E16" s="2">
+        <v>32</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" s="2">
+        <v>512</v>
+      </c>
+      <c r="J16" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="3">
+        <v>10400</v>
+      </c>
+      <c r="L16">
+        <v>400</v>
+      </c>
+      <c r="M16">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>